<commit_message>
Message Controller + SCRUM Backlog update
Added many methods and began work on posting comments. Updated the SCRUM backlog to make our Sprint planning meeting easier later today.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM_Backlogs.xlsx
+++ b/Documentation/SCRUM_Backlogs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBB76DF-6ADF-4AC5-8EAC-64AD5DA42A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746E6243-8BDF-442E-A308-15B68A786DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1080" windowWidth="17472" windowHeight="9876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1968" yWindow="1428" windowWidth="17472" windowHeight="9876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -80,36 +80,18 @@
     <t>Sprint Backlog (Tasks)</t>
   </si>
   <si>
-    <t>As a registered user I want to set-up a personal profile page to present myself.</t>
-  </si>
-  <si>
     <t>estimated</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>User Story ID</t>
   </si>
   <si>
-    <t>User can define and view profile page with profile picture and self description.</t>
-  </si>
-  <si>
     <t>Effort (hours)</t>
   </si>
   <si>
-    <t>in process</t>
-  </si>
-  <si>
-    <t>to do</t>
-  </si>
-  <si>
     <t>Persons</t>
   </si>
   <si>
-    <t>accepted</t>
-  </si>
-  <si>
     <t>Improve user profile functionality</t>
   </si>
   <si>
@@ -252,6 +234,36 @@
   </si>
   <si>
     <t>Comment Posting- Create error checking inside any SPROCs or Triggers in the database</t>
+  </si>
+  <si>
+    <t>By visiting localhost:8080 the website should be displayed. The website should be pleasing to the eye and have no glaring issues.</t>
+  </si>
+  <si>
+    <t>By successfully joining or creating a session a user should be automatically redirected to the session page. The page should be pleasing to the eyes and have no glaring issues.</t>
+  </si>
+  <si>
+    <t>A user will be correctly indentified as a member or a session owner and the session page HTML and layout will change based on the user type.</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Users will be able to post comments and have them appear on the page at least locally. Comments will persist even if the page is refreshed.</t>
+  </si>
+  <si>
+    <t>Users will see there comment under the comment of another user and formatted in a way that distinguishes it from a regular non-reply comment. The reply will persist after page refresh even if it's just local.</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Users will be able to see other users comments formatted onto the page. The comments will be in the order that they we posted and new comments will be displayed on the page without having to manually refresh the page.</t>
+  </si>
+  <si>
+    <t>A user can like a message</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -404,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +467,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -462,11 +483,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -476,20 +518,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -497,6 +530,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -506,32 +542,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,50 +873,50 @@
     <col min="2" max="2" width="74.109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="5" width="11.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="6" max="6" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -901,7 +925,7 @@
         <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -909,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -918,7 +942,7 @@
         <v>75</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -926,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -935,7 +959,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -943,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -952,7 +976,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -960,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -969,7 +993,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -977,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -986,7 +1010,7 @@
         <v>75</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -994,7 +1018,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -1011,7 +1035,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -1028,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -1045,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -1062,7 +1086,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -1079,7 +1103,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
@@ -1096,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1113,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -1130,7 +1154,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -1147,7 +1171,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -1164,7 +1188,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
@@ -1181,7 +1205,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -1193,18 +1217,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2">
-        <f>SUM(D3:D21)</f>
-        <v>702</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="8" t="s">
-        <v>27</v>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2">
+        <f>SUM(D3:D22)</f>
+        <v>706</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1223,17 +1264,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="50.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="45" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="22" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="10" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" style="10" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" style="10" customWidth="1"/>
@@ -1271,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1286,144 +1327,175 @@
       <c r="B8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="45">
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="45">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="45">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="45">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="45">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="E18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="44">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="44">
-        <v>2</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="44">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="C19" s="21">
+        <v>1</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -1432,13 +1504,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="44">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="C20" s="21">
+        <v>2</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -1447,12 +1519,12 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="44">
+        <v>43</v>
+      </c>
+      <c r="C21" s="21">
         <v>3</v>
       </c>
       <c r="D21" s="11"/>
@@ -1462,12 +1534,12 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="44">
+        <v>44</v>
+      </c>
+      <c r="C22" s="21">
         <v>3</v>
       </c>
       <c r="D22" s="11"/>
@@ -1477,12 +1549,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="44">
+        <v>45</v>
+      </c>
+      <c r="C23" s="21">
         <v>3</v>
       </c>
       <c r="D23" s="11"/>
@@ -1492,12 +1564,12 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="44">
+        <v>46</v>
+      </c>
+      <c r="C24" s="21">
         <v>3</v>
       </c>
       <c r="D24" s="11"/>
@@ -1507,12 +1579,12 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="44">
+        <v>47</v>
+      </c>
+      <c r="C25" s="21">
         <v>3</v>
       </c>
       <c r="D25" s="11"/>
@@ -1522,13 +1594,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="44">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="21">
+        <v>3</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -1537,13 +1609,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="44">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="C27" s="21">
+        <v>3</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -1552,13 +1624,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="44">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="C28" s="21">
+        <v>2</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -1567,12 +1639,12 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="44">
+        <v>51</v>
+      </c>
+      <c r="C29" s="21">
         <v>4</v>
       </c>
       <c r="D29" s="11"/>
@@ -1582,13 +1654,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="44">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="C30" s="21">
+        <v>4</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -1597,13 +1669,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="44">
-        <v>5</v>
+        <v>53</v>
+      </c>
+      <c r="C31" s="21">
+        <v>4</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -1612,13 +1684,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="44">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="C32" s="21">
+        <v>6</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
@@ -1627,12 +1699,12 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="44">
+        <v>59</v>
+      </c>
+      <c r="C33" s="21">
         <v>5</v>
       </c>
       <c r="D33" s="11"/>
@@ -1642,13 +1714,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="44">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="C34" s="21">
+        <v>5</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -1657,13 +1729,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="44">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="C35" s="21">
+        <v>5</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -1672,12 +1744,12 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="44">
+        <v>55</v>
+      </c>
+      <c r="C36" s="21">
         <v>6</v>
       </c>
       <c r="D36" s="11"/>
@@ -1687,13 +1759,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="44">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="C37" s="21">
+        <v>6</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -1702,13 +1774,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="44">
-        <v>3</v>
+        <v>57</v>
+      </c>
+      <c r="C38" s="21">
+        <v>6</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -1717,12 +1789,12 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="44">
+        <v>61</v>
+      </c>
+      <c r="C39" s="21">
         <v>3</v>
       </c>
       <c r="D39" s="11"/>
@@ -1732,13 +1804,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="45">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="C40" s="21">
+        <v>3</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -1747,13 +1819,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="45">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C41" s="21">
+        <v>3</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
@@ -1762,12 +1834,12 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="45">
+        <v>64</v>
+      </c>
+      <c r="C42" s="22">
         <v>4</v>
       </c>
       <c r="D42" s="11"/>
@@ -1777,10 +1849,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>27</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="44"/>
+        <v>25</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="22">
+        <v>4</v>
+      </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
@@ -1788,63 +1864,92 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>28</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="44"/>
+        <v>26</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="22">
+        <v>4</v>
+      </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="40"/>
+      <c r="A45" s="3">
+        <v>27</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
+      <c r="A46" s="3">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="40"/>
+      <c r="A47" s="20"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="40"/>
+      <c r="A48" s="20"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="40"/>
+      <c r="A49" s="20"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="40"/>
+      <c r="A50" s="20"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="40"/>
+      <c r="A51" s="20"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="40"/>
+      <c r="A52" s="20"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="40"/>
+      <c r="A53" s="20"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="40"/>
+      <c r="A54" s="20"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="40"/>
+      <c r="A55" s="20"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="40"/>
+      <c r="A56" s="20"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G15:G16"/>
+  <mergeCells count="13">
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1912,12 +2017,12 @@
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="15" t="s">
         <v>3</v>
       </c>
@@ -1925,19 +2030,19 @@
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1952,10 +2057,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1970,32 +2075,32 @@
       <c r="B15" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="39" t="s">
         <v>18</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -2251,16 +2356,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>